<commit_message>
Updated file reading and model
</commit_message>
<xml_diff>
--- a/data/14 Day Predictions.xlsx
+++ b/data/14 Day Predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\homeassistant_tracker_predictor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A343FF0-F6AD-43A0-93FD-CC6A2B610BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498CF3E1-2F79-4AFA-B685-B6387A452132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{9BA59B83-7F70-4E96-B8BA-DB5845AC3BA5}"/>
+    <workbookView xWindow="-75" yWindow="10380" windowWidth="38520" windowHeight="10260" activeTab="1" xr2:uid="{9BA59B83-7F70-4E96-B8BA-DB5845AC3BA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -541,7 +541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20E12D9-6AA1-4CE9-8C4B-1D89A8E70B9A}">
   <dimension ref="A1:I625"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
@@ -19199,8 +19199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AFF9C4-00AB-4CE3-975D-921F2B6B550F}">
   <dimension ref="A1:AN25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AN8" sqref="AN8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19527,13 +19527,6 @@
       <c r="AL3">
         <v>12.108147000000001</v>
       </c>
-      <c r="AM3">
-        <f>(AL3*1.2012)+10.3059</f>
-        <v>24.8502061764</v>
-      </c>
-      <c r="AN3">
-        <v>24.02</v>
-      </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -19686,13 +19679,6 @@
       <c r="AL4">
         <v>7.2037909999999998</v>
       </c>
-      <c r="AM4">
-        <f t="shared" ref="AM4:AM15" si="0">(AL4*1.2012)+10.3059</f>
-        <v>18.959093749200001</v>
-      </c>
-      <c r="AN4">
-        <v>24.35</v>
-      </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -19845,10 +19831,6 @@
       <c r="AL5">
         <v>10.051444999999999</v>
       </c>
-      <c r="AM5">
-        <f t="shared" si="0"/>
-        <v>22.379695733999998</v>
-      </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -20001,9 +19983,8 @@
       <c r="AL6">
         <v>9.0311260000000004</v>
       </c>
-      <c r="AM6">
-        <f t="shared" si="0"/>
-        <v>21.154088551200001</v>
+      <c r="AN6">
+        <v>23.46</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
@@ -20158,8 +20139,10 @@
         <v>7.2665790000000001</v>
       </c>
       <c r="AM7">
-        <f t="shared" si="0"/>
-        <v>19.034514694800002</v>
+        <v>20.149999999999999</v>
+      </c>
+      <c r="AN7">
+        <v>21.69</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
@@ -20314,8 +20297,7 @@
         <v>9.8992880000000003</v>
       </c>
       <c r="AM8">
-        <f t="shared" si="0"/>
-        <v>22.196924745600001</v>
+        <v>16.62</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
@@ -20470,8 +20452,7 @@
         <v>10.282747000000001</v>
       </c>
       <c r="AM9">
-        <f t="shared" si="0"/>
-        <v>22.6575356964</v>
+        <v>22.29</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
@@ -20626,8 +20607,7 @@
         <v>10.813575999999999</v>
       </c>
       <c r="AM10">
-        <f t="shared" si="0"/>
-        <v>23.295167491199997</v>
+        <v>33.1</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
@@ -20782,8 +20762,7 @@
         <v>10.242599</v>
       </c>
       <c r="AM11">
-        <f t="shared" si="0"/>
-        <v>22.609309918800001</v>
+        <v>21.78</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
@@ -20938,8 +20917,7 @@
         <v>10.186241000000001</v>
       </c>
       <c r="AM12">
-        <f t="shared" si="0"/>
-        <v>22.541612689200001</v>
+        <v>20.149999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
@@ -21094,8 +21072,7 @@
         <v>10.092615</v>
       </c>
       <c r="AM13">
-        <f t="shared" si="0"/>
-        <v>22.429149138</v>
+        <v>18.34</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
@@ -21250,8 +21227,7 @@
         <v>8.2062989999999996</v>
       </c>
       <c r="AM14">
-        <f t="shared" si="0"/>
-        <v>20.1633063588</v>
+        <v>18.62</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
@@ -21406,8 +21382,7 @@
         <v>8.5338360000000009</v>
       </c>
       <c r="AM15">
-        <f t="shared" si="0"/>
-        <v>20.5567438032</v>
+        <v>18.59</v>
       </c>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">

</xml_diff>